<commit_message>
boot strapping + correlation plots HFT
</commit_message>
<xml_diff>
--- a/clockshift/metadata_file.xlsx
+++ b/clockshift/metadata_file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
   <si>
     <t>filename</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>2024-07-03_D_e_evenbiggerbox</t>
+  </si>
+  <si>
+    <t>2024-07-18_C_e</t>
+  </si>
+  <si>
+    <t>2024-07-18_D_e</t>
+  </si>
+  <si>
+    <t>2024-07-18_E_e</t>
   </si>
 </sst>
 </file>
@@ -465,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +705,7 @@
         <v>13</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -909,7 +918,7 @@
         <v>29</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1014,7 +1023,7 @@
         <v>21</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1034,7 +1043,8 @@
         <v>0.1</v>
       </c>
       <c r="F16">
-        <v>1.2699999999999999E-2</v>
+        <f>(0.0127+0.0133)/2</f>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="G16">
         <v>47</v>
@@ -1084,7 +1094,7 @@
         <v>21</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1154,7 +1164,7 @@
         <v>21</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1189,6 +1199,111 @@
         <v>21</v>
       </c>
       <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>0.82</v>
+      </c>
+      <c r="D21">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E21">
+        <v>0.15</v>
+      </c>
+      <c r="F21">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="G21">
+        <v>47</v>
+      </c>
+      <c r="H21">
+        <v>202.1</v>
+      </c>
+      <c r="I21">
+        <v>47.215899999999998</v>
+      </c>
+      <c r="J21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>0.82</v>
+      </c>
+      <c r="D22">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E22">
+        <v>0.2</v>
+      </c>
+      <c r="F22">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="G22">
+        <v>47</v>
+      </c>
+      <c r="H22">
+        <v>202.1</v>
+      </c>
+      <c r="I22">
+        <v>47.215899999999998</v>
+      </c>
+      <c r="J22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>0.82</v>
+      </c>
+      <c r="D23">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E23">
+        <v>0.2</v>
+      </c>
+      <c r="F23">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="G23">
+        <v>47</v>
+      </c>
+      <c r="H23">
+        <v>202.1</v>
+      </c>
+      <c r="I23">
+        <v>47.215899999999998</v>
+      </c>
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rf spectrum and other general scripts
</commit_message>
<xml_diff>
--- a/clockshift/metadata_file.xlsx
+++ b/clockshift/metadata_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\UNOBTAINIUM\E_Carmen_Santiago\Analysis Scripts\analysis\clockshift\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Analysis Scripts\analysis\clockshift\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
   <si>
     <t>filename</t>
   </si>
@@ -162,22 +162,65 @@
   </si>
   <si>
     <t>EF_sem</t>
+  </si>
+  <si>
+    <t>2024-09-10_P_e</t>
+  </si>
+  <si>
+    <t>2024-09-11_C_e</t>
+  </si>
+  <si>
+    <t>2024-09-11_F_e</t>
+  </si>
+  <si>
+    <t>2024-09-11_H_e</t>
+  </si>
+  <si>
+    <t>2024-09-11_J_e</t>
+  </si>
+  <si>
+    <t>2024-09-12_E_e</t>
+  </si>
+  <si>
+    <t>2024-09-10_L_e</t>
+  </si>
+  <si>
+    <t>barnu</t>
+  </si>
+  <si>
+    <t>trap_depth</t>
+  </si>
+  <si>
+    <t>2024-09-18_F_e</t>
+  </si>
+  <si>
+    <t>2024-09-18_K_e</t>
+  </si>
+  <si>
+    <t>2024-09-23_H_e</t>
+  </si>
+  <si>
+    <t>2024-09-24_C_e</t>
+  </si>
+  <si>
+    <t>2024-09-23_J_e</t>
+  </si>
+  <si>
+    <t>Tshots/2</t>
+  </si>
+  <si>
+    <t>Tshots</t>
+  </si>
+  <si>
+    <t>Ushots/2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -205,17 +248,972 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="136">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -490,74 +1488,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R27"/>
+  <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" t="s">
         <v>10</v>
       </c>
+      <c r="T1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V1" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
@@ -573,43 +1590,58 @@
         <v>0.2</v>
       </c>
       <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>352</v>
+      </c>
+      <c r="H2">
         <v>32741.974026</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>9664.85968815858</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>0.44160199999999999</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>0.10303</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>1.6E-2</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>1.7212429999999999E-3</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>47</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>202.1</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>47.215899999999998</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2">
+      <c r="S2">
         <v>1</v>
       </c>
-      <c r="R2" s="2"/>
+      <c r="T2">
+        <f>H2/2</f>
+        <v>16370.987013</v>
+      </c>
+      <c r="U2">
+        <v>72676</v>
+      </c>
+      <c r="V2">
+        <f t="shared" ref="V2:V34" si="0">U2/2</f>
+        <v>36338</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
@@ -625,42 +1657,57 @@
         <v>0.1</v>
       </c>
       <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3">
+        <v>352</v>
+      </c>
+      <c r="H3">
         <v>18526.304166999998</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2285.7418931423499</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>0.29538399999999998</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>2.4240000000000001E-2</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>5.4832700000000004E-4</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>47</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>202.1</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>47.215899999999998</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2"/>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T35" si="1">H3/2</f>
+        <v>9263.1520834999992</v>
+      </c>
+      <c r="U3">
+        <v>61124</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="0"/>
+        <v>30562</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -677,43 +1724,60 @@
         <v>0.05</v>
       </c>
       <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4">
+        <v>352</v>
+      </c>
+      <c r="H4">
         <v>16912.769230999998</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>1095.03288843101</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.32753900000000002</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>2.1099E-2</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>2.7969399999999998E-4</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>47</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>202.1</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>47.215899999999998</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="R4" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="S4">
         <v>1</v>
       </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>8456.3846154999992</v>
+      </c>
+      <c r="U4">
+        <v>66932</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="0"/>
+        <v>33466</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -730,41 +1794,57 @@
         <v>0.3</v>
       </c>
       <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5">
+        <v>352</v>
+      </c>
+      <c r="H5">
         <v>16912.769230999998</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>1095.03288843101</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>0.32753900000000002</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>2.1099E-2</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>2.7969399999999998E-4</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>47</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>202.1</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>47.215899999999998</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="2">
+      <c r="S5">
         <v>1</v>
       </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>8456.3846154999992</v>
+      </c>
+      <c r="U5">
+        <v>66932</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="0"/>
+        <v>33466</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -780,26 +1860,43 @@
       <c r="E6">
         <v>0.05</v>
       </c>
-      <c r="J6">
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>352</v>
+      </c>
+      <c r="L6">
         <v>1.6E-2</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>47</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>202.1</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>47.215899999999998</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>13</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>1</v>
       </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>67686</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="0"/>
+        <v>33843</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -816,40 +1913,57 @@
         <v>0.1</v>
       </c>
       <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7">
+        <v>352</v>
+      </c>
+      <c r="H7">
         <v>38973.816278999999</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>2256.9510242834299</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>0.53736700000000004</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>1.1523E-2</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>3.2877299999999998E-4</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>47</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>202.1</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>47.215899999999998</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>21</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>1</v>
       </c>
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>19486.908139499999</v>
+      </c>
+      <c r="U7">
+        <v>55960</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>27980</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -866,40 +1980,57 @@
         <v>0.1</v>
       </c>
       <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8">
+        <v>352</v>
+      </c>
+      <c r="H8">
         <v>54043.633332999998</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>1358.3049708695301</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>0.51547100000000001</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>1.3211000000000001E-2</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>1.9E-2</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>1.6083300000000001E-4</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>47</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>202.1</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>47.215899999999998</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
         <v>21</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>0</v>
       </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>27021.816666499999</v>
+      </c>
+      <c r="U8">
+        <v>74073</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>37036.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -916,40 +2047,57 @@
         <v>0.1</v>
       </c>
       <c r="F9">
+        <v>0.1</v>
+      </c>
+      <c r="G9">
+        <v>352</v>
+      </c>
+      <c r="H9">
         <v>54043.633332999998</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>1358.3049708695301</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>0.51547100000000001</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>1.3211000000000001E-2</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>1.9E-2</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>1.6083300000000001E-4</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>47</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>202.1</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>47.215899999999998</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>21</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>1</v>
       </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>27021.816666499999</v>
+      </c>
+      <c r="U9">
+        <v>74073</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="0"/>
+        <v>37036.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -966,40 +2114,57 @@
         <v>0.1</v>
       </c>
       <c r="F10">
+        <v>0.1</v>
+      </c>
+      <c r="G10">
+        <v>352</v>
+      </c>
+      <c r="H10">
         <v>54043.633332999998</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>1358.3049708695301</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>0.51547100000000001</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>1.3211000000000001E-2</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>1.9E-2</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>1.6083300000000001E-4</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>47</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>202.1</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>47.215899999999998</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>21</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>1</v>
       </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>27021.816666499999</v>
+      </c>
+      <c r="U10">
+        <v>74073</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="0"/>
+        <v>37036.5</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1016,43 +2181,60 @@
         <v>0.05</v>
       </c>
       <c r="F11">
+        <v>0.1</v>
+      </c>
+      <c r="G11">
+        <v>352</v>
+      </c>
+      <c r="H11">
         <v>54043.633332999998</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>1358.3049708695301</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>0.51547100000000001</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>1.3211000000000001E-2</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>1.9E-2</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>1.6083300000000001E-4</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>47</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>202.1</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>47.215899999999998</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>21</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>26</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>1</v>
       </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>27021.816666499999</v>
+      </c>
+      <c r="U11">
+        <v>74073</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="0"/>
+        <v>37036.5</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1069,40 +2251,57 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="F12">
+        <v>0.1</v>
+      </c>
+      <c r="G12">
+        <v>352</v>
+      </c>
+      <c r="H12">
         <v>54043.633332999998</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>1358.3049708695301</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>0.51547100000000001</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>1.3211000000000001E-2</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>1.9E-2</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>1.6083300000000001E-4</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>47</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>202.1</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>47.215899999999998</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>21</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>0</v>
       </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>27021.816666499999</v>
+      </c>
+      <c r="U12">
+        <v>74073</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="0"/>
+        <v>37036.5</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1119,40 +2318,57 @@
         <v>0.05</v>
       </c>
       <c r="F13">
+        <v>0.1</v>
+      </c>
+      <c r="G13">
+        <v>352</v>
+      </c>
+      <c r="H13">
         <v>47547.977778</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>2211.0713256889599</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>0.53050299999999995</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>1.1075E-2</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>2.8498100000000001E-4</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>47</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>202.1</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>47.215899999999998</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>21</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>1</v>
       </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>23773.988889</v>
+      </c>
+      <c r="U13">
+        <v>57589</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="0"/>
+        <v>28794.5</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1169,40 +2385,57 @@
         <v>0.05</v>
       </c>
       <c r="F14">
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <v>352</v>
+      </c>
+      <c r="H14">
         <v>47547.977778</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>2211.0713256889599</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>0.53050299999999995</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>1.1075E-2</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>2.8498100000000001E-4</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>47</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>202.1</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>47.215899999999998</v>
       </c>
-      <c r="O14" t="s">
+      <c r="Q14" t="s">
         <v>29</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>1</v>
       </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>23773.988889</v>
+      </c>
+      <c r="U14">
+        <v>57589</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="0"/>
+        <v>28794.5</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1219,40 +2452,57 @@
         <v>0.1</v>
       </c>
       <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15">
+        <v>352</v>
+      </c>
+      <c r="H15">
         <v>47547.977778</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>2211.0713256889599</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>0.53050299999999995</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>1.1075E-2</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>2.8498100000000001E-4</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>47</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>202.1</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>47.215899999999998</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>21</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>1</v>
       </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>23773.988889</v>
+      </c>
+      <c r="U15">
+        <v>57589</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="0"/>
+        <v>28794.5</v>
+      </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1269,40 +2519,57 @@
         <v>0.05</v>
       </c>
       <c r="F16">
+        <v>0.1</v>
+      </c>
+      <c r="G16">
+        <v>352</v>
+      </c>
+      <c r="H16">
         <v>16424.465217000001</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>559.34882295995897</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>0.24734600000000001</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>1.0743000000000001E-2</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>1.29E-2</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>1.44721E-4</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>47</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>202.1</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>47.215899999999998</v>
       </c>
-      <c r="O16" t="s">
+      <c r="Q16" t="s">
         <v>21</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>1</v>
       </c>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>8212.2326085000004</v>
+      </c>
+      <c r="U16">
+        <v>79495</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="0"/>
+        <v>39747.5</v>
+      </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1319,40 +2586,57 @@
         <v>0.1</v>
       </c>
       <c r="F17">
+        <v>0.1</v>
+      </c>
+      <c r="G17">
+        <v>352</v>
+      </c>
+      <c r="H17">
         <v>16424.465217000001</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>559.34882295995897</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>0.24734600000000001</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>1.0743000000000001E-2</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>1.29E-2</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>1.44721E-4</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>47</v>
       </c>
-      <c r="M17">
+      <c r="O17">
         <v>202.1</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>47.215899999999998</v>
       </c>
-      <c r="O17" t="s">
+      <c r="Q17" t="s">
         <v>21</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>1</v>
       </c>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>8212.2326085000004</v>
+      </c>
+      <c r="U17">
+        <v>79495</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="0"/>
+        <v>39747.5</v>
+      </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1369,40 +2653,57 @@
         <v>0.1</v>
       </c>
       <c r="F18">
+        <v>0.1</v>
+      </c>
+      <c r="G18">
+        <v>352</v>
+      </c>
+      <c r="H18">
         <v>29006.269090999998</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>10595.3093103225</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>0.42105999999999999</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>8.0463999999999994E-2</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>1.9743909999999998E-3</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>47</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>202.1</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>47.215899999999998</v>
       </c>
-      <c r="O18" t="s">
+      <c r="Q18" t="s">
         <v>21</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <v>1</v>
       </c>
+      <c r="T18">
+        <f t="shared" si="1"/>
+        <v>14503.134545499999</v>
+      </c>
+      <c r="U18">
+        <v>57313</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="0"/>
+        <v>28656.5</v>
+      </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1419,40 +2720,57 @@
         <v>0.1</v>
       </c>
       <c r="F19">
+        <v>0.1</v>
+      </c>
+      <c r="G19">
+        <v>352</v>
+      </c>
+      <c r="H19">
         <v>29006.269090999998</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>10595.3093103225</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>0.42105999999999999</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>8.0463999999999994E-2</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>1.9743909999999998E-3</v>
       </c>
-      <c r="L19">
+      <c r="N19">
         <v>47</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>202.1</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>47.215899999999998</v>
       </c>
-      <c r="O19" t="s">
+      <c r="Q19" t="s">
         <v>21</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>1</v>
       </c>
+      <c r="T19">
+        <f t="shared" si="1"/>
+        <v>14503.134545499999</v>
+      </c>
+      <c r="U19">
+        <v>57313</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="0"/>
+        <v>28656.5</v>
+      </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1469,40 +2787,57 @@
         <v>0.1</v>
       </c>
       <c r="F20">
+        <v>0.1</v>
+      </c>
+      <c r="G20">
+        <v>352</v>
+      </c>
+      <c r="H20">
         <v>29006.269090999998</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>10595.3093103225</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>0.42105999999999999</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>8.0463999999999994E-2</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>1.9743909999999998E-3</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>47</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <v>202.1</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <v>47.215899999999998</v>
       </c>
-      <c r="O20" t="s">
+      <c r="Q20" t="s">
         <v>21</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <v>0</v>
       </c>
+      <c r="T20">
+        <f t="shared" si="1"/>
+        <v>14503.134545499999</v>
+      </c>
+      <c r="U20">
+        <v>57313</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="0"/>
+        <v>28656.5</v>
+      </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1519,40 +2854,57 @@
         <v>0.15</v>
       </c>
       <c r="F21">
+        <v>0.1</v>
+      </c>
+      <c r="G21">
+        <v>352</v>
+      </c>
+      <c r="H21">
         <v>16465.798332999999</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>2373.4353251838402</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>0.40073399999999998</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>5.8556999999999998E-2</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>1.29E-2</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>6.3346699999999997E-4</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>47</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>202.1</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>47.215899999999998</v>
       </c>
-      <c r="O21" t="s">
+      <c r="Q21" t="s">
         <v>21</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <v>0</v>
       </c>
+      <c r="T21">
+        <f t="shared" si="1"/>
+        <v>8232.8991664999994</v>
+      </c>
+      <c r="U21">
+        <v>58266</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="0"/>
+        <v>29133</v>
+      </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1569,40 +2921,57 @@
         <v>0.2</v>
       </c>
       <c r="F22">
+        <v>0.1</v>
+      </c>
+      <c r="G22">
+        <v>352</v>
+      </c>
+      <c r="H22">
         <v>16465.798332999999</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>2373.4353251838402</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>0.40073399999999998</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>5.8556999999999998E-2</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>1.29E-2</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>6.3346699999999997E-4</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>47</v>
       </c>
-      <c r="M22">
+      <c r="O22">
         <v>202.1</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>47.215899999999998</v>
       </c>
-      <c r="O22" t="s">
+      <c r="Q22" t="s">
         <v>21</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <v>0</v>
       </c>
+      <c r="T22">
+        <f t="shared" si="1"/>
+        <v>8232.8991664999994</v>
+      </c>
+      <c r="U22">
+        <v>58266</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="0"/>
+        <v>29133</v>
+      </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1619,41 +2988,859 @@
         <v>0.2</v>
       </c>
       <c r="F23">
+        <v>0.1</v>
+      </c>
+      <c r="G23">
+        <v>352</v>
+      </c>
+      <c r="H23">
         <v>16465.798332999999</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <v>2373.4353251838402</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>0.40073399999999998</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>5.8556999999999998E-2</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>1.29E-2</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>6.3346699999999997E-4</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>47</v>
       </c>
-      <c r="M23">
+      <c r="O23">
         <v>202.1</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>47.215899999999998</v>
       </c>
-      <c r="O23" t="s">
+      <c r="Q23" t="s">
         <v>21</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <v>0</v>
       </c>
+      <c r="T23">
+        <f t="shared" si="1"/>
+        <v>8232.8991664999994</v>
+      </c>
+      <c r="U23">
+        <v>58266</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="0"/>
+        <v>29133</v>
+      </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>1.02</v>
+      </c>
+      <c r="D24">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0.1</v>
+      </c>
+      <c r="G24">
+        <v>312</v>
+      </c>
+      <c r="H24">
+        <v>36057</v>
+      </c>
+      <c r="I24">
+        <v>1100</v>
+      </c>
+      <c r="J24">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="K24">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="L24">
+        <v>1.49E-2</v>
+      </c>
+      <c r="M24">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="N24">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O24">
+        <v>202.14</v>
+      </c>
+      <c r="P24">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>21</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="1"/>
+        <v>18028.5</v>
+      </c>
+      <c r="U24">
+        <v>83240</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="0"/>
+        <v>41620</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>1.02</v>
+      </c>
+      <c r="D25">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0.1</v>
+      </c>
+      <c r="G25">
+        <v>312</v>
+      </c>
+      <c r="H25">
+        <v>36057</v>
+      </c>
+      <c r="I25">
+        <v>1100</v>
+      </c>
+      <c r="J25">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="K25">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="L25">
+        <v>1.49E-2</v>
+      </c>
+      <c r="M25">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="N25">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O25">
+        <v>202.14</v>
+      </c>
+      <c r="P25">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="1"/>
+        <v>18028.5</v>
+      </c>
+      <c r="U25">
+        <v>83240</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="0"/>
+        <v>41620</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>0.93</v>
+      </c>
+      <c r="D26">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0.1</v>
+      </c>
+      <c r="G26">
+        <v>312</v>
+      </c>
+      <c r="H26">
+        <v>36057</v>
+      </c>
+      <c r="I26">
+        <v>1100</v>
+      </c>
+      <c r="J26">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="K26">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="L26">
+        <v>1.49E-2</v>
+      </c>
+      <c r="M26">
+        <v>1.6000000000000001E-4</v>
+      </c>
+      <c r="N26">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O26">
+        <v>202.14</v>
+      </c>
+      <c r="P26">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>21</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="1"/>
+        <v>18028.5</v>
+      </c>
+      <c r="U26">
+        <v>76914</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="0"/>
+        <v>38457</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>0.93</v>
+      </c>
+      <c r="D27">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="G27">
+        <v>312</v>
+      </c>
+      <c r="H27">
+        <v>55201</v>
+      </c>
+      <c r="I27">
+        <v>600</v>
+      </c>
+      <c r="J27">
+        <v>0.442</v>
+      </c>
+      <c r="K27">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="L27">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="M27">
+        <v>6.4000000000000005E-4</v>
+      </c>
+      <c r="N27">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O27">
+        <v>202.14</v>
+      </c>
+      <c r="P27">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>21</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="1"/>
+        <v>27600.5</v>
+      </c>
+      <c r="U27">
+        <v>76914</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="0"/>
+        <v>38457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>0.93</v>
+      </c>
+      <c r="D28">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0.15</v>
+      </c>
+      <c r="G28">
+        <v>377</v>
+      </c>
+      <c r="H28">
+        <v>54029</v>
+      </c>
+      <c r="I28">
+        <v>380</v>
+      </c>
+      <c r="J28">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="K28">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="L28">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="M28">
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="N28">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O28">
+        <v>202.14</v>
+      </c>
+      <c r="P28">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>21</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="1"/>
+        <v>27014.5</v>
+      </c>
+      <c r="U28">
+        <v>76914</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="0"/>
+        <v>38457</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>0.93</v>
+      </c>
+      <c r="D29">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0.15</v>
+      </c>
+      <c r="G29">
+        <v>377</v>
+      </c>
+      <c r="H29">
+        <v>54029</v>
+      </c>
+      <c r="I29">
+        <v>380</v>
+      </c>
+      <c r="J29">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="K29">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="L29">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="M29">
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="N29">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O29">
+        <v>202.14</v>
+      </c>
+      <c r="P29">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="1"/>
+        <v>27014.5</v>
+      </c>
+      <c r="U29">
+        <v>76914</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="0"/>
+        <v>38457</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>0.93</v>
+      </c>
+      <c r="D30">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0.15</v>
+      </c>
+      <c r="G30">
+        <v>377</v>
+      </c>
+      <c r="H30">
+        <v>35301</v>
+      </c>
+      <c r="I30">
+        <v>3900</v>
+      </c>
+      <c r="J30">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="K30">
+        <v>2.8E-3</v>
+      </c>
+      <c r="L30">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="M30">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="N30">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O30">
+        <v>202.14</v>
+      </c>
+      <c r="P30">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>21</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="1"/>
+        <v>17650.5</v>
+      </c>
+      <c r="U30">
+        <v>68286</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="0"/>
+        <v>34143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>0.93</v>
+      </c>
+      <c r="D31">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0.15</v>
+      </c>
+      <c r="G31">
+        <v>377</v>
+      </c>
+      <c r="H31">
+        <v>40333</v>
+      </c>
+      <c r="I31">
+        <v>880</v>
+      </c>
+      <c r="J31">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="K31">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="L31">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="M31">
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="N31">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O31">
+        <v>202.14</v>
+      </c>
+      <c r="P31">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>21</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="1"/>
+        <v>20166.5</v>
+      </c>
+      <c r="U31">
+        <v>70608</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="0"/>
+        <v>35304</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>0.93</v>
+      </c>
+      <c r="D32">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0.15</v>
+      </c>
+      <c r="G32">
+        <v>377</v>
+      </c>
+      <c r="H32">
+        <v>25124</v>
+      </c>
+      <c r="I32">
+        <v>350</v>
+      </c>
+      <c r="J32">
+        <v>0.45</v>
+      </c>
+      <c r="K32">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="L32">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="M32">
+        <v>7.2999999999999996E-4</v>
+      </c>
+      <c r="N32">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O32">
+        <v>202.14</v>
+      </c>
+      <c r="P32">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>21</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="1"/>
+        <v>12562</v>
+      </c>
+      <c r="U32">
+        <v>70608</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="0"/>
+        <v>35304</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>0.93</v>
+      </c>
+      <c r="D33">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0.15</v>
+      </c>
+      <c r="G33">
+        <v>377</v>
+      </c>
+      <c r="H33">
+        <v>45614</v>
+      </c>
+      <c r="I33">
+        <v>540</v>
+      </c>
+      <c r="J33">
+        <v>0.53</v>
+      </c>
+      <c r="K33">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="L33">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="M33">
+        <v>7.6999999999999996E-4</v>
+      </c>
+      <c r="N33">
+        <v>46.22</v>
+      </c>
+      <c r="O33">
+        <v>202.14</v>
+      </c>
+      <c r="P33">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>21</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="1"/>
+        <v>22807</v>
+      </c>
+      <c r="U33">
+        <v>63143</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="0"/>
+        <v>31571.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>0.93</v>
+      </c>
+      <c r="D34">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0.15</v>
+      </c>
+      <c r="G34">
+        <v>377</v>
+      </c>
+      <c r="H34">
+        <v>22687</v>
+      </c>
+      <c r="I34">
+        <v>420</v>
+      </c>
+      <c r="J34">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="K34">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="L34">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="M34">
+        <v>9.6000000000000002E-4</v>
+      </c>
+      <c r="N34">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O34">
+        <v>202.14</v>
+      </c>
+      <c r="P34">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>21</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="1"/>
+        <v>11343.5</v>
+      </c>
+      <c r="U34">
+        <v>63143</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="0"/>
+        <v>31571.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>0.93</v>
+      </c>
+      <c r="D35">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0.15</v>
+      </c>
+      <c r="G35">
+        <v>377</v>
+      </c>
+      <c r="H35">
+        <v>45110</v>
+      </c>
+      <c r="I35">
+        <v>440</v>
+      </c>
+      <c r="J35">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="K35">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L35">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="M35">
+        <v>6.4000000000000005E-4</v>
+      </c>
+      <c r="N35">
+        <v>46.222700000000003</v>
+      </c>
+      <c r="O35">
+        <v>202.14</v>
+      </c>
+      <c r="P35">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>21</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="1"/>
+        <v>22555</v>
+      </c>
+      <c r="U35">
+        <v>61154</v>
+      </c>
+      <c r="V35">
+        <f>U35/2</f>
+        <v>30577</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>